<commit_message>
Added album covers, merged Billboard data
</commit_message>
<xml_diff>
--- a/Data/billboard.xlsx
+++ b/Data/billboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zayne\GitRepos\SufjanSentiment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976077D-D614-4BE1-AD75-10FD476AAE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFA9B49-D6FA-43D3-98B1-2F8295901E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30150" yWindow="2475" windowWidth="25755" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,16 +48,16 @@
     <t>peak_date</t>
   </si>
   <si>
-    <t>weeks</t>
-  </si>
-  <si>
-    <t>Age of Adz</t>
-  </si>
-  <si>
     <t>All Delighted People</t>
   </si>
   <si>
     <t>The Avalanche</t>
+  </si>
+  <si>
+    <t>The Age of Adz</t>
+  </si>
+  <si>
+    <t>weeks_on</t>
   </si>
 </sst>
 </file>
@@ -379,12 +379,14 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -398,7 +400,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -431,7 +433,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -445,7 +447,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>27</v>
@@ -459,7 +461,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>71</v>

</xml_diff>